<commit_message>
Add table of results
</commit_message>
<xml_diff>
--- a/Results/Evaluation_Proposal/Evaluation.xlsx
+++ b/Results/Evaluation_Proposal/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\Documents\Thesis\FeatSubSpace GAN\FSS_GAN\Results\Evaluation_Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D37B569-D63B-43E7-A364-BFE237837195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7E79B0-5543-49EA-9EB0-358F413A406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="6" xr2:uid="{7CBD0493-6410-48D5-83A7-33CA8C9F6410}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="2" activeTab="12" xr2:uid="{7CBD0493-6410-48D5-83A7-33CA8C9F6410}"/>
   </bookViews>
   <sheets>
     <sheet name="Deep SVDD Paper Params" sheetId="36" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="135">
   <si>
     <t>Seed</t>
   </si>
@@ -583,6 +583,30 @@
        0,18966636, 0,20476414, 0,1641334 , 0,34711707, 0,65465295,
        0,48577434, 0,7262061 , 0,12351393, 0,32504538, 0,72112066,
        0,5062771 , 0,13790222]</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Std deviation</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>std dev</t>
   </si>
 </sst>
 </file>
@@ -670,11 +694,12 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="80">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
+        <strike val="0"/>
       </font>
     </dxf>
     <dxf>
@@ -744,67 +769,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -833,13 +797,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1300,15 +1257,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{05C3F970-0077-4958-98FA-8A25277BFCDB}" name="Tabelle_Internet_ads" displayName="Tabelle_Internet_ads" ref="A1:I6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I6" xr:uid="{05C3F970-0077-4958-98FA-8A25277BFCDB}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2E4C27E6-1884-446E-82B3-D97EA723EA57}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{9403AA73-CEBB-44CD-B894-8E9760E3F3BC}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{29DFBBBE-8647-4035-82A2-943CEEC79038}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{9A1E5B6F-6C6F-4813-B9F5-C12063AF85B0}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{02618EBF-882E-482C-BADB-0A427AC74206}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{0BB271AD-5E3E-4EDD-B502-7071E2D9D683}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{7C2AFCCB-C191-47C9-BF2B-AC2429B9261C}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{96538A87-FF70-4BAB-B909-990CE3402E46}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{75921241-7FB7-45E8-9C16-9D9D0850E414}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{2E4C27E6-1884-446E-82B3-D97EA723EA57}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{9403AA73-CEBB-44CD-B894-8E9760E3F3BC}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{29DFBBBE-8647-4035-82A2-943CEEC79038}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{9A1E5B6F-6C6F-4813-B9F5-C12063AF85B0}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{02618EBF-882E-482C-BADB-0A427AC74206}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{0BB271AD-5E3E-4EDD-B502-7071E2D9D683}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{7C2AFCCB-C191-47C9-BF2B-AC2429B9261C}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{96538A87-FF70-4BAB-B909-990CE3402E46}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{75921241-7FB7-45E8-9C16-9D9D0850E414}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1318,15 +1275,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C74785AA-0498-449F-AB20-ECA8752778DE}" name="Tabelle_Arrythmia" displayName="Tabelle_Arrythmia" ref="A1:I6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I6" xr:uid="{C74785AA-0498-449F-AB20-ECA8752778DE}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FBFB8C22-591C-4941-93E7-646A6C5BFE1B}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{08EFB349-0BF6-419B-BA8E-33D8DA880511}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{BB8CC07C-E48F-4059-AC54-4D42BE98B9F3}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{6E2885C3-6AB1-49CD-B8D9-69149543E7C2}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{C382980E-0952-4ED5-9CF4-C6F7499225A9}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{708D498E-93ED-4231-9D45-28283FD96D4F}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{58DA6648-5CF9-46D5-A23A-E44069AE950B}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{61A06D48-30BA-44C7-97B9-A281D3B4276D}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{B828E2E9-5956-4EF2-B285-4F01F217EB55}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{FBFB8C22-591C-4941-93E7-646A6C5BFE1B}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{08EFB349-0BF6-419B-BA8E-33D8DA880511}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{BB8CC07C-E48F-4059-AC54-4D42BE98B9F3}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{6E2885C3-6AB1-49CD-B8D9-69149543E7C2}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{C382980E-0952-4ED5-9CF4-C6F7499225A9}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{708D498E-93ED-4231-9D45-28283FD96D4F}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{58DA6648-5CF9-46D5-A23A-E44069AE950B}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{61A06D48-30BA-44C7-97B9-A281D3B4276D}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{B828E2E9-5956-4EF2-B285-4F01F217EB55}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1336,16 +1293,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{EA337558-3934-44CF-BADE-63F3E4129B7A}" name="Tabelle_Fashion_MNIST" displayName="Tabelle_Fashion_MNIST" ref="A1:J69" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:J69" xr:uid="{EA337558-3934-44CF-BADE-63F3E4129B7A}"/>
   <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{6954C7B3-C478-4BA5-8B29-3493D4C27DEE}" uniqueName="11" name="Seed" queryTableFieldId="11" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{968EAB8A-E7E5-45F4-8329-383ADAF5FC8B}" uniqueName="12" name="Class" queryTableFieldId="12" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{1E84610C-CADE-4B1A-8C26-5CEFF55E802A}" uniqueName="13" name="LOF_AUC" queryTableFieldId="13" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{07FFC098-5B52-495C-9F0F-43931F614510}" uniqueName="14" name="LOF_50" queryTableFieldId="14" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{26D663AB-3BF2-4736-83BA-D3278BC364F9}" uniqueName="15" name="LOF_100" queryTableFieldId="15" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{15B0D585-1EB2-4AB5-8442-ADCBFE6A46CB}" uniqueName="16" name="LOF_500" queryTableFieldId="16" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{5DBEA6F7-8E89-4096-A7C5-CC9BE27F15A9}" uniqueName="17" name="KNN_AUC" queryTableFieldId="17" dataDxfId="36"/>
-    <tableColumn id="18" xr3:uid="{4C807E74-9293-487E-8974-A873C18A2D3B}" uniqueName="18" name="MO_GAAL_AUC" queryTableFieldId="18" dataDxfId="35"/>
-    <tableColumn id="19" xr3:uid="{540B9E4E-2280-4D4C-A04B-E38C9AB2565B}" uniqueName="19" name="AnoGAN_AUC" queryTableFieldId="19" dataDxfId="34"/>
-    <tableColumn id="20" xr3:uid="{77B6FEAD-6311-4528-9C3F-893B34427E0A}" uniqueName="20" name="DeepSVDD_AUC" queryTableFieldId="20" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{6954C7B3-C478-4BA5-8B29-3493D4C27DEE}" uniqueName="11" name="Seed" queryTableFieldId="11" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{968EAB8A-E7E5-45F4-8329-383ADAF5FC8B}" uniqueName="12" name="Class" queryTableFieldId="12" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{1E84610C-CADE-4B1A-8C26-5CEFF55E802A}" uniqueName="13" name="LOF_AUC" queryTableFieldId="13" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{07FFC098-5B52-495C-9F0F-43931F614510}" uniqueName="14" name="LOF_50" queryTableFieldId="14" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{26D663AB-3BF2-4736-83BA-D3278BC364F9}" uniqueName="15" name="LOF_100" queryTableFieldId="15" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{15B0D585-1EB2-4AB5-8442-ADCBFE6A46CB}" uniqueName="16" name="LOF_500" queryTableFieldId="16" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{5DBEA6F7-8E89-4096-A7C5-CC9BE27F15A9}" uniqueName="17" name="KNN_AUC" queryTableFieldId="17" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{4C807E74-9293-487E-8974-A873C18A2D3B}" uniqueName="18" name="MO_GAAL_AUC" queryTableFieldId="18" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{540B9E4E-2280-4D4C-A04B-E38C9AB2565B}" uniqueName="19" name="AnoGAN_AUC" queryTableFieldId="19" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{77B6FEAD-6311-4528-9C3F-893B34427E0A}" uniqueName="20" name="DeepSVDD_AUC" queryTableFieldId="20" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1355,16 +1312,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42BBA015-EEFD-442A-A6DA-57538788572A}" name="Tabelle_Cifar10" displayName="Tabelle_Cifar10" ref="A1:J69" tableType="queryTable">
   <autoFilter ref="A1:J69" xr:uid="{42BBA015-EEFD-442A-A6DA-57538788572A}"/>
   <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{2DAC05A1-69E1-457E-B566-E6F424463B0C}" uniqueName="11" name="Seed" queryTableFieldId="11" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{8D17398B-379B-4526-969B-9B32DC577B09}" uniqueName="12" name="Class" queryTableFieldId="12" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{12FD2422-9156-4E18-B58B-0A3CB4450ED9}" uniqueName="13" name="LOF_AUC" queryTableFieldId="13" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{4FD8C035-4CFB-4C33-8BEB-BB00CAA4F595}" uniqueName="14" name="LOF_50" queryTableFieldId="14" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{926466E1-7504-470C-8681-BAA8735EE9A0}" uniqueName="15" name="LOF_100" queryTableFieldId="15" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{E7279FC6-1BE3-4337-98EE-1F89D9CA6F5D}" uniqueName="16" name="LOF_500" queryTableFieldId="16" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{02348F09-C540-48D3-99C9-A7412C9D3170}" uniqueName="17" name="KNN_AUC" queryTableFieldId="17" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{8E78C03D-9472-41C8-93CB-CD693C71057C}" uniqueName="18" name="MO_GAAL_AUC" queryTableFieldId="18" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{77762A02-BED4-47A8-AF0D-A1ADF5814A40}" uniqueName="19" name="AnoGAN_AUC" queryTableFieldId="19" dataDxfId="23"/>
-    <tableColumn id="20" xr3:uid="{674FEE22-6779-40E7-933B-BC267867D384}" uniqueName="20" name="DeepSVDD_AUC" queryTableFieldId="20" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{2DAC05A1-69E1-457E-B566-E6F424463B0C}" uniqueName="11" name="Seed" queryTableFieldId="11" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{8D17398B-379B-4526-969B-9B32DC577B09}" uniqueName="12" name="Class" queryTableFieldId="12" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{12FD2422-9156-4E18-B58B-0A3CB4450ED9}" uniqueName="13" name="LOF_AUC" queryTableFieldId="13" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{4FD8C035-4CFB-4C33-8BEB-BB00CAA4F595}" uniqueName="14" name="LOF_50" queryTableFieldId="14" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{926466E1-7504-470C-8681-BAA8735EE9A0}" uniqueName="15" name="LOF_100" queryTableFieldId="15" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{E7279FC6-1BE3-4337-98EE-1F89D9CA6F5D}" uniqueName="16" name="LOF_500" queryTableFieldId="16" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{02348F09-C540-48D3-99C9-A7412C9D3170}" uniqueName="17" name="KNN_AUC" queryTableFieldId="17" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{8E78C03D-9472-41C8-93CB-CD693C71057C}" uniqueName="18" name="MO_GAAL_AUC" queryTableFieldId="18" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{77762A02-BED4-47A8-AF0D-A1ADF5814A40}" uniqueName="19" name="AnoGAN_AUC" queryTableFieldId="19" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{674FEE22-6779-40E7-933B-BC267867D384}" uniqueName="20" name="DeepSVDD_AUC" queryTableFieldId="20" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1484,9 +1441,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16D51B30-7F05-470D-9961-EA28424CC4FF}" name="Tabelle_Params_8_C__2" displayName="Tabelle_Params_8_C__2" ref="A1:C16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C16" xr:uid="{16D51B30-7F05-470D-9961-EA28424CC4FF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9CC0DF13-8514-4636-BA6A-DDD5108186E0}" uniqueName="1" name="Learning rate generator" queryTableFieldId="1" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{0B2B3B78-90A4-4497-BB54-018B808E70D5}" uniqueName="2" name=" Stop epochs" queryTableFieldId="2" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{AB2A3DFA-9955-4D37-A5D0-DA6113635B01}" uniqueName="3" name=" Average AUC" queryTableFieldId="3" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{9CC0DF13-8514-4636-BA6A-DDD5108186E0}" uniqueName="1" name="Learning rate generator" queryTableFieldId="1" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{0B2B3B78-90A4-4497-BB54-018B808E70D5}" uniqueName="2" name=" Stop epochs" queryTableFieldId="2" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{AB2A3DFA-9955-4D37-A5D0-DA6113635B01}" uniqueName="3" name=" Average AUC" queryTableFieldId="3" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1496,9 +1453,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{170B6A86-370E-4A9A-9BDD-A2ACAC3683C9}" name="Tabelle_Params_6_C" displayName="Tabelle_Params_6_C" ref="A1:C16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C16" xr:uid="{170B6A86-370E-4A9A-9BDD-A2ACAC3683C9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BF192353-C4CF-4900-ACE3-6FFC76F2AE14}" uniqueName="1" name="Learning rate generator" queryTableFieldId="1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{0E8B7269-86A6-47A3-97B7-FEA7819EA4FE}" uniqueName="2" name=" Stop epochs" queryTableFieldId="2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{0BA52A74-4EBA-4E3C-8853-E659ACE282BA}" uniqueName="3" name=" Average AUC" queryTableFieldId="3" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{BF192353-C4CF-4900-ACE3-6FFC76F2AE14}" uniqueName="1" name="Learning rate generator" queryTableFieldId="1" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{0E8B7269-86A6-47A3-97B7-FEA7819EA4FE}" uniqueName="2" name=" Stop epochs" queryTableFieldId="2" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{0BA52A74-4EBA-4E3C-8853-E659ACE282BA}" uniqueName="3" name=" Average AUC" queryTableFieldId="3" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1508,9 +1465,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6D5F3E8C-6048-4C25-B0BA-D78A0D893B69}" name="Tabelle_Params_8_F" displayName="Tabelle_Params_8_F" ref="A1:C10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{6D5F3E8C-6048-4C25-B0BA-D78A0D893B69}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DF658CBC-9E9C-4B3B-B186-A335925EBC8B}" uniqueName="1" name="Learning rate" queryTableFieldId="1" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{84D6BF6D-FA36-451F-BFC7-1151B9AC3BC4}" uniqueName="2" name=" Epochs" queryTableFieldId="2" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{D85B33C5-4620-4760-9F6A-7EF47C966D14}" uniqueName="3" name=" AUC" queryTableFieldId="3" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{DF658CBC-9E9C-4B3B-B186-A335925EBC8B}" uniqueName="1" name="Learning rate" queryTableFieldId="1" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{84D6BF6D-FA36-451F-BFC7-1151B9AC3BC4}" uniqueName="2" name=" Epochs" queryTableFieldId="2" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{D85B33C5-4620-4760-9F6A-7EF47C966D14}" uniqueName="3" name=" AUC" queryTableFieldId="3" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1520,9 +1477,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E1CE0FB1-85D1-4CAD-AD1F-351FA092DE05}" name="Tabelle_Params_8_C" displayName="Tabelle_Params_8_C" ref="A1:C10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{E1CE0FB1-85D1-4CAD-AD1F-351FA092DE05}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{18FB1400-2EA6-403A-82E8-D571163DE0EE}" uniqueName="1" name="Learning rate" queryTableFieldId="1" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{1704C863-A1A1-4943-87E9-EC18D51002BD}" uniqueName="2" name="Epochs" queryTableFieldId="2" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{B021868B-3D95-4DED-A449-D4A71B1F8208}" uniqueName="3" name="AUC" queryTableFieldId="3" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{18FB1400-2EA6-403A-82E8-D571163DE0EE}" uniqueName="1" name="Learning rate" queryTableFieldId="1" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{1704C863-A1A1-4943-87E9-EC18D51002BD}" uniqueName="2" name="Epochs" queryTableFieldId="2" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{B021868B-3D95-4DED-A449-D4A71B1F8208}" uniqueName="3" name="AUC" queryTableFieldId="3" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1532,15 +1489,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E58C0CC5-D536-40A0-B988-704FB5C805DC}" name="Tabelle_Waveform" displayName="Tabelle_Waveform" ref="A1:I6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I6" xr:uid="{E58C0CC5-D536-40A0-B988-704FB5C805DC}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{8289C0FF-5EA1-48B8-AF28-D0BE4FE241B2}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{F8882AAC-A0CD-4270-97B4-2EA86FE23790}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{1C2DCD26-C941-4C9E-974A-41B070573265}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{E298157B-D206-432D-A214-5A0DC72C75A4}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{F1F5543C-2FCD-4B48-89CF-12C8BF9576A7}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{06F37020-D871-4EAE-A53F-3BF9CCBAE1F3}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{234B5464-E3EA-4489-B102-FD46100889EB}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{4985C673-30EA-4C5A-A523-B8891E762E91}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{D5EB49AF-F5A8-418B-9CC9-5902EAD1795E}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{8289C0FF-5EA1-48B8-AF28-D0BE4FE241B2}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{F8882AAC-A0CD-4270-97B4-2EA86FE23790}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{1C2DCD26-C941-4C9E-974A-41B070573265}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{E298157B-D206-432D-A214-5A0DC72C75A4}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{F1F5543C-2FCD-4B48-89CF-12C8BF9576A7}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{06F37020-D871-4EAE-A53F-3BF9CCBAE1F3}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{234B5464-E3EA-4489-B102-FD46100889EB}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{4985C673-30EA-4C5A-A523-B8891E762E91}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{D5EB49AF-F5A8-418B-9CC9-5902EAD1795E}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1550,15 +1507,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4ADB7DFC-93AD-47EA-8763-F99729EBD4E8}" name="Tabelle_Spambase" displayName="Tabelle_Spambase" ref="A1:I6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I6" xr:uid="{4ADB7DFC-93AD-47EA-8763-F99729EBD4E8}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0CDD8384-0F2F-4E74-82C3-97B572EB8E60}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{89D7D86A-7452-4DEC-A563-6A0223F3BCDF}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{2D0AD5CC-106B-4391-826B-0389D6FCDAA2}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{1D390C9C-8A30-4674-B15C-04BDB1D4A3F1}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{74E3A22C-A6E9-4FF3-85DF-B5ED71AC5B53}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{6ED07410-70C5-4ABD-9AEB-E6C240552587}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{9ABD5DEC-EEA5-4E33-BAC5-4485A672C10C}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{6B9D5E9F-235E-4875-835E-67DE3EE516AE}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{33A65136-9D38-428D-A7B6-BF3EE35FA9D2}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{0CDD8384-0F2F-4E74-82C3-97B572EB8E60}" uniqueName="1" name="Seed" queryTableFieldId="1" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{89D7D86A-7452-4DEC-A563-6A0223F3BCDF}" uniqueName="2" name="LOF_AUC" queryTableFieldId="2" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{2D0AD5CC-106B-4391-826B-0389D6FCDAA2}" uniqueName="3" name="LOF_50" queryTableFieldId="3" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{1D390C9C-8A30-4674-B15C-04BDB1D4A3F1}" uniqueName="4" name="LOF_100" queryTableFieldId="4" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{74E3A22C-A6E9-4FF3-85DF-B5ED71AC5B53}" uniqueName="5" name="LOF_500" queryTableFieldId="5" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{6ED07410-70C5-4ABD-9AEB-E6C240552587}" uniqueName="6" name="KNN_AUC" queryTableFieldId="6" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{9ABD5DEC-EEA5-4E33-BAC5-4485A672C10C}" uniqueName="7" name="MO_GAAL_AUC" queryTableFieldId="7" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{6B9D5E9F-235E-4875-835E-67DE3EE516AE}" uniqueName="8" name="AnoGAN_AUC" queryTableFieldId="8" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{33A65136-9D38-428D-A7B6-BF3EE35FA9D2}" uniqueName="9" name="Deep_SVDD_AUC" queryTableFieldId="9" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2077,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C841215E-ABDB-4B9A-8F7B-BBAAA96E7330}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,9 +2223,120 @@
         <v>0.76074585419273999</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(Tabelle_Internet_ads[LOF_AUC])</f>
+        <v>0.84973404255319096</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(Tabelle_Internet_ads[LOF_50])</f>
+        <v>0.80918335419274035</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(Tabelle_Internet_ads[LOF_100])</f>
+        <v>0.80556163954943671</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(Tabelle_Internet_ads[LOF_500])</f>
+        <v>0.80964877972465532</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(Tabelle_Internet_ads[KNN_AUC])</f>
+        <v>0.825455647684605</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(Tabelle_Internet_ads[MO_GAAL_AUC])</f>
+        <v>0.34875625782227737</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(Tabelle_Internet_ads[AnoGAN_AUC])</f>
+        <v>0.49213861076345378</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(Tabelle_Internet_ads[Deep_SVDD_AUC])</f>
+        <v>0.77622418648310343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <f>MEDIAN(Tabelle_Internet_ads[LOF_AUC])</f>
+        <v>0.84973404255319096</v>
+      </c>
+      <c r="C9">
+        <f>MEDIAN(Tabelle_Internet_ads[LOF_50])</f>
+        <v>0.81275422403003705</v>
+      </c>
+      <c r="D9">
+        <f>MEDIAN(Tabelle_Internet_ads[LOF_100])</f>
+        <v>0.80561639549436803</v>
+      </c>
+      <c r="E9">
+        <f>MEDIAN(Tabelle_Internet_ads[LOF_500])</f>
+        <v>0.810387984981226</v>
+      </c>
+      <c r="F9">
+        <f>MEDIAN(Tabelle_Internet_ads[KNN_AUC])</f>
+        <v>0.825455647684605</v>
+      </c>
+      <c r="G9">
+        <f>MEDIAN(Tabelle_Internet_ads[MO_GAAL_AUC])</f>
+        <v>0.34079709011263998</v>
+      </c>
+      <c r="H9">
+        <f>MEDIAN(Tabelle_Internet_ads[AnoGAN_AUC])</f>
+        <v>0.47324780976220199</v>
+      </c>
+      <c r="I9">
+        <f>MEDIAN(Tabelle_Internet_ads[Deep_SVDD_AUC])</f>
+        <v>0.77239127033792199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[LOF_AUC])</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[LOF_50])</f>
+        <v>9.9974422120631037E-3</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[LOF_100])</f>
+        <v>7.9659924598066197E-3</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[LOF_500])</f>
+        <v>2.9243251214622567E-3</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[KNN_AUC])</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[MO_GAAL_AUC])</f>
+        <v>2.8022164043290877E-2</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[AnoGAN_AUC])</f>
+        <v>5.158904732502919E-2</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.STDEV.S(Tabelle_Internet_ads[Deep_SVDD_AUC])</f>
+        <v>1.8361335457473954E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:I6">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>B2=MAX($B2:$I2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2281,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15A12F8-3249-43C7-AB07-6D3262B6FDE4}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,9 +2536,120 @@
         <v>0.455942622950819</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(Tabelle_Arrythmia[LOF_AUC])</f>
+        <v>0.72950819672131095</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(Tabelle_Arrythmia[LOF_50])</f>
+        <v>0.73381147540983571</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(Tabelle_Arrythmia[LOF_100])</f>
+        <v>0.73565573770491755</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(Tabelle_Arrythmia[LOF_500])</f>
+        <v>0.73606557377049131</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(Tabelle_Arrythmia[KNN_AUC])</f>
+        <v>0.72643442622950805</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(Tabelle_Arrythmia[MO_GAAL_AUC])</f>
+        <v>0.63975409836065522</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(Tabelle_Arrythmia[AnoGAN_AUC])</f>
+        <v>0.56885245901639292</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(Tabelle_Arrythmia[Deep_SVDD_AUC])</f>
+        <v>0.50655737704917958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9">
+        <f>MEDIAN(Tabelle_Arrythmia[LOF_AUC])</f>
+        <v>0.72950819672131095</v>
+      </c>
+      <c r="C9">
+        <f>MEDIAN(Tabelle_Arrythmia[LOF_50])</f>
+        <v>0.73155737704918</v>
+      </c>
+      <c r="D9">
+        <f>MEDIAN(Tabelle_Arrythmia[LOF_100])</f>
+        <v>0.73565573770491799</v>
+      </c>
+      <c r="E9">
+        <f>MEDIAN(Tabelle_Arrythmia[LOF_500])</f>
+        <v>0.73668032786885196</v>
+      </c>
+      <c r="F9">
+        <f>MEDIAN(Tabelle_Arrythmia[KNN_AUC])</f>
+        <v>0.72643442622950805</v>
+      </c>
+      <c r="G9">
+        <f>MEDIAN(Tabelle_Arrythmia[MO_GAAL_AUC])</f>
+        <v>0.62192622950819598</v>
+      </c>
+      <c r="H9">
+        <f>MEDIAN(Tabelle_Arrythmia[AnoGAN_AUC])</f>
+        <v>0.56352459016393397</v>
+      </c>
+      <c r="I9">
+        <f>MEDIAN(Tabelle_Arrythmia[Deep_SVDD_AUC])</f>
+        <v>0.455942622950819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[LOF_AUC])</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[LOF_50])</f>
+        <v>7.6467656381330462E-3</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[LOF_100])</f>
+        <v>3.1579989769309692E-3</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[LOF_500])</f>
+        <v>2.1246353845622268E-3</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[KNN_AUC])</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[MO_GAAL_AUC])</f>
+        <v>9.1167224441769723E-2</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[AnoGAN_AUC])</f>
+        <v>0.12591917155614465</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.STDEV.S(Tabelle_Arrythmia[Deep_SVDD_AUC])</f>
+        <v>0.12840449102859636</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:I6">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>B2=MAX($B2:$I2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2483,10 +2662,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F8EA0B-F2CE-4ED2-97FA-905DCA7505CD}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C111" sqref="A72:C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4135,9 +4314,1164 @@
         <v>0.696265111111111</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73">
+        <f>AVERAGE(C2:C6)</f>
+        <v>0.97799766666666588</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ref="D73:J73" si="0">AVERAGE(D2:D6)</f>
+        <v>0.97877633333333303</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="0"/>
+        <v>0.97871402222222181</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="0"/>
+        <v>0.97854733333333288</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="0"/>
+        <v>0.96541199999999905</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="0"/>
+        <v>2.2295066666666596E-2</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="0"/>
+        <v>0.33597954444444378</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="0"/>
+        <v>0.89835306666666592</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74">
+        <f>MEDIAN(C2:C6)</f>
+        <v>0.97799766666666599</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ref="D74:J74" si="1">MEDIAN(D2:D6)</f>
+        <v>0.97873522222222198</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>0.97861655555555505</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>0.97852644444444403</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>0.96541199999999905</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>2.27993888888888E-2</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="1"/>
+        <v>0.32052466666666601</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>0.90910688888888802</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>134</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:J75" si="2">_xlfn.STDEV.S(D2:D6)</f>
+        <v>2.2528510057980876E-4</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="2"/>
+        <v>1.8961662751977435E-4</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="2"/>
+        <v>7.7599955453491376E-5</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="2"/>
+        <v>4.3832677275403055E-3</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="2"/>
+        <v>9.7637918966712409E-2</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="2"/>
+        <v>1.912408524599252E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77">
+        <f>AVERAGE(C9:C13)</f>
+        <v>0.8132747777777769</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77:J77" si="3">AVERAGE(D9:D13)</f>
+        <v>0.81752199999999919</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>0.81724088888888868</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>0.81707613333333262</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="3"/>
+        <v>0.87934777777777706</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="3"/>
+        <v>0.27280547777777742</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="3"/>
+        <v>0.39067524444444401</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="3"/>
+        <v>0.56087066666666618</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>133</v>
+      </c>
+      <c r="C78">
+        <f>MEDIAN(C9:C13)</f>
+        <v>0.81327477777777701</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ref="D78:J78" si="4">MEDIAN(D9:D13)</f>
+        <v>0.81689888888888795</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="4"/>
+        <v>0.81713422222222198</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="4"/>
+        <v>0.81701688888888802</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>0.87934777777777695</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="4"/>
+        <v>0.275903055555555</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="4"/>
+        <v>0.376559166666666</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="4"/>
+        <v>0.57126311111111105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79">
+        <f>_xlfn.STDEV.S(C9:C13)</f>
+        <v>1.2412670766236366E-16</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ref="D79:J79" si="5">_xlfn.STDEV.S(D9:D13)</f>
+        <v>1.11718871986926E-3</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="5"/>
+        <v>7.6417224239659252E-4</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="5"/>
+        <v>2.2505279764630412E-4</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>1.2412670766236366E-16</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="5"/>
+        <v>9.7110390021319694E-3</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="5"/>
+        <v>4.1044736864513563E-2</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="5"/>
+        <v>4.0295476025062699E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81">
+        <f>AVERAGE(C16:C20)</f>
+        <v>0.96752133333333301</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ref="D81:J81" si="6">AVERAGE(D16:D20)</f>
+        <v>0.96793693333333297</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>0.96790762222222182</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="6"/>
+        <v>0.96791873333333278</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="6"/>
+        <v>0.98460966666666605</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="6"/>
+        <v>0.10981984444444404</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="6"/>
+        <v>0.62236107777777738</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="6"/>
+        <v>0.9447877111111106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82">
+        <f>MEDIAN(C16:C20)</f>
+        <v>0.96752133333333301</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ref="D82:J82" si="7">MEDIAN(D16:D20)</f>
+        <v>0.96784966666666605</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="7"/>
+        <v>0.96789455555555504</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="7"/>
+        <v>0.96792255555555495</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="7"/>
+        <v>0.98460966666666605</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="7"/>
+        <v>0.103258444444444</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="7"/>
+        <v>0.49738027777777699</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="7"/>
+        <v>0.94551188888888804</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83">
+        <f>_xlfn.STDEV.S(C16:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <f t="shared" ref="D83:J83" si="8">_xlfn.STDEV.S(D16:D20)</f>
+        <v>2.130777201277238E-4</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="8"/>
+        <v>1.5899653696047698E-4</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="8"/>
+        <v>1.2408579270159786E-5</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="8"/>
+        <v>1.4831693466855082E-2</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="8"/>
+        <v>0.18845052482520325</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="8"/>
+        <v>4.4365487054398856E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85">
+        <f>AVERAGE(C23:C27)</f>
+        <v>0.80383455555555516</v>
+      </c>
+      <c r="D85">
+        <f t="shared" ref="D85:J85" si="9">AVERAGE(D23:D27)</f>
+        <v>0.80562473333333284</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="9"/>
+        <v>0.80575317777777733</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="9"/>
+        <v>0.80565922222222197</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="9"/>
+        <v>0.82768255555555503</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="9"/>
+        <v>0.3412611777777772</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="9"/>
+        <v>0.47917146666666621</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="9"/>
+        <v>0.60406697777777718</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>133</v>
+      </c>
+      <c r="C86">
+        <f>MEDIAN(C23:C27)</f>
+        <v>0.80383455555555505</v>
+      </c>
+      <c r="D86">
+        <f t="shared" ref="D86:J86" si="10">MEDIAN(D23:D27)</f>
+        <v>0.80545377777777705</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="10"/>
+        <v>0.80582899999999902</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="10"/>
+        <v>0.80567500000000003</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="10"/>
+        <v>0.82768255555555503</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="10"/>
+        <v>0.33860888888888802</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="10"/>
+        <v>0.42648622222222199</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="10"/>
+        <v>0.60535866666666605</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <f t="shared" ref="D87:J87" si="11">_xlfn.STDEV.S(D23:D27)</f>
+        <v>4.8900300814532318E-4</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="11"/>
+        <v>3.3976788191355828E-4</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="11"/>
+        <v>8.1779853536374043E-5</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="11"/>
+        <v>1.1681489494397257E-2</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="11"/>
+        <v>0.1146197725762306</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="11"/>
+        <v>3.4137305618055024E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89">
+        <f>AVERAGE(C30:C34)</f>
+        <v>0.89150133333333303</v>
+      </c>
+      <c r="D89">
+        <f t="shared" ref="D89:J89" si="12">AVERAGE(D30:D34)</f>
+        <v>0.89322691111111063</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="12"/>
+        <v>0.89338302222222166</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="12"/>
+        <v>0.89344826666666621</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="12"/>
+        <v>0.90747588888888797</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="12"/>
+        <v>0.6758197666666661</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="12"/>
+        <v>0.63087609999999961</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="12"/>
+        <v>0.84483152222222202</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90">
+        <f>MEDIAN(C30:C34)</f>
+        <v>0.89150133333333303</v>
+      </c>
+      <c r="D90">
+        <f t="shared" ref="D90:J90" si="13">MEDIAN(D30:D34)</f>
+        <v>0.89321222222222196</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="13"/>
+        <v>0.89318933333333295</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="13"/>
+        <v>0.89348366666666601</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="13"/>
+        <v>0.90747588888888797</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="13"/>
+        <v>0.68153227777777703</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="13"/>
+        <v>0.79320933333333299</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="13"/>
+        <v>0.84925016666666597</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91">
+        <f>_xlfn.STDEV.S(C30:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <f t="shared" ref="D91:J91" si="14">_xlfn.STDEV.S(D30:D34)</f>
+        <v>3.4925812379538569E-4</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="14"/>
+        <v>3.3483597790375289E-4</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="14"/>
+        <v>2.2949689473159834E-4</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="14"/>
+        <v>2.7582613090277684E-2</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="14"/>
+        <v>0.30041851008887943</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="14"/>
+        <v>2.7646057906581839E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>132</v>
+      </c>
+      <c r="C93">
+        <f>AVERAGE(C37:C41)</f>
+        <v>0.91303022222222197</v>
+      </c>
+      <c r="D93">
+        <f t="shared" ref="D93:J93" si="15">AVERAGE(D37:D41)</f>
+        <v>0.91364275555555496</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="15"/>
+        <v>0.91361637777777727</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="15"/>
+        <v>0.91350895555555522</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="15"/>
+        <v>0.90349166666666603</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="15"/>
+        <v>0.1695473888888884</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="15"/>
+        <v>0.25067737777777721</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="15"/>
+        <v>0.71562629999999938</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>133</v>
+      </c>
+      <c r="C94">
+        <f>MEDIAN(C37:C41)</f>
+        <v>0.91303022222222197</v>
+      </c>
+      <c r="D94">
+        <f t="shared" ref="D94:J94" si="16">MEDIAN(D37:D41)</f>
+        <v>0.91372933333333295</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="16"/>
+        <v>0.91366155555555495</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="16"/>
+        <v>0.91350055555555498</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="16"/>
+        <v>0.90349166666666603</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="16"/>
+        <v>0.17050605555555501</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="16"/>
+        <v>0.24036288888888799</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="16"/>
+        <v>0.71383177777777695</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95">
+        <f>_xlfn.STDEV.S(C37:C41)</f>
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <f t="shared" ref="D95:J95" si="17">_xlfn.STDEV.S(D37:D41)</f>
+        <v>1.477229931868797E-4</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="17"/>
+        <v>2.39376641598869E-4</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="17"/>
+        <v>5.1342026680869811E-5</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="17"/>
+        <v>1.4157563449028571E-2</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="17"/>
+        <v>1.9817264281024045E-2</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="17"/>
+        <v>2.5009629269296684E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97">
+        <f>AVERAGE(C44:C48)</f>
+        <v>0.901905333333333</v>
+      </c>
+      <c r="D97">
+        <f t="shared" ref="D97:J97" si="18">AVERAGE(D44:D48)</f>
+        <v>0.90230831111111043</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="18"/>
+        <v>0.90238139999999945</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="18"/>
+        <v>0.90242948888888874</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="18"/>
+        <v>0.94027611111111098</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="18"/>
+        <v>0.25477933333333258</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="18"/>
+        <v>0.50427705555555524</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="18"/>
+        <v>0.84963787777777733</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>133</v>
+      </c>
+      <c r="C98">
+        <f>MEDIAN(C44:C48)</f>
+        <v>0.901905333333333</v>
+      </c>
+      <c r="D98">
+        <f t="shared" ref="D98:J98" si="19">MEDIAN(D44:D48)</f>
+        <v>0.90243899999999899</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="19"/>
+        <v>0.90244144444444396</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="19"/>
+        <v>0.90242144444444405</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="19"/>
+        <v>0.94027611111111098</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="19"/>
+        <v>0.25284938888888803</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="19"/>
+        <v>0.49802744444444402</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="19"/>
+        <v>0.84814683333333296</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99">
+        <f>_xlfn.STDEV.S(C44:C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <f t="shared" ref="D99:J99" si="20">_xlfn.STDEV.S(D44:D48)</f>
+        <v>5.0719551104067115E-4</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="20"/>
+        <v>3.9868034319422808E-4</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="20"/>
+        <v>9.9645718100737509E-5</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="20"/>
+        <v>1.5701730154923085E-2</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="20"/>
+        <v>4.8536718713980707E-2</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="20"/>
+        <v>2.8288698502741814E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>132</v>
+      </c>
+      <c r="C101">
+        <f>AVERAGE(C51:C55)</f>
+        <v>0.85463877777777708</v>
+      </c>
+      <c r="D101">
+        <f t="shared" ref="D101:J101" si="21">AVERAGE(D51:D55)</f>
+        <v>0.85685491111111067</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="21"/>
+        <v>0.85650195555555531</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="21"/>
+        <v>0.85679406666666613</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="21"/>
+        <v>0.89499083333333296</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="21"/>
+        <v>0.2491716555555552</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="21"/>
+        <v>0.33799275555555519</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="21"/>
+        <v>0.69606357777777739</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>133</v>
+      </c>
+      <c r="C102">
+        <f>MEDIAN(C51:C55)</f>
+        <v>0.85463877777777697</v>
+      </c>
+      <c r="D102">
+        <f t="shared" ref="D102:J102" si="22">MEDIAN(D51:D55)</f>
+        <v>0.85646733333333303</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="22"/>
+        <v>0.85632333333333299</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="22"/>
+        <v>0.85673333333333301</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="22"/>
+        <v>0.89499083333333296</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="22"/>
+        <v>0.24799861111111099</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="22"/>
+        <v>0.35065005555555501</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="22"/>
+        <v>0.66911299999999996</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>134</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <f t="shared" ref="D103:J103" si="23">_xlfn.STDEV.S(D51:D55)</f>
+        <v>7.1657131751565401E-4</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="23"/>
+        <v>7.0881060435044722E-4</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="23"/>
+        <v>2.3586595900506083E-4</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="23"/>
+        <v>7.1854206836001024E-3</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="23"/>
+        <v>5.0715750995762365E-2</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="23"/>
+        <v>6.5347220659411592E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>132</v>
+      </c>
+      <c r="C105">
+        <f>AVERAGE(C58:C62)</f>
+        <v>0.95288522222222194</v>
+      </c>
+      <c r="D105">
+        <f t="shared" ref="D105:J105" si="24">AVERAGE(D58:D62)</f>
+        <v>0.95359266666666609</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="24"/>
+        <v>0.95344948888888847</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="24"/>
+        <v>0.95360537777777721</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="24"/>
+        <v>0.98867644444444402</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="24"/>
+        <v>0.25978296666666645</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="24"/>
+        <v>0.59924713333333268</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="24"/>
+        <v>0.93618768888888848</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>133</v>
+      </c>
+      <c r="C106">
+        <f>MEDIAN(C58:C62)</f>
+        <v>0.95288522222222205</v>
+      </c>
+      <c r="D106">
+        <f t="shared" ref="D106:J106" si="25">MEDIAN(D58:D62)</f>
+        <v>0.95372511111111102</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="25"/>
+        <v>0.95341177777777697</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="25"/>
+        <v>0.95358877777777695</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="25"/>
+        <v>0.98867644444444402</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="25"/>
+        <v>0.27209749999999999</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="25"/>
+        <v>0.50308188888888805</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="25"/>
+        <v>0.93400066666666604</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>134</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <f t="shared" ref="D107:J107" si="26">_xlfn.STDEV.S(D58:D62)</f>
+        <v>2.0270904466813104E-4</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="26"/>
+        <v>1.6145395704956659E-4</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="26"/>
+        <v>1.6606659752895715E-4</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="26"/>
+        <v>2.0741595138657771E-2</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="26"/>
+        <v>0.17752165183547611</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="26"/>
+        <v>1.4751925568264088E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>132</v>
+      </c>
+      <c r="C109">
+        <f>AVERAGE(C65:C69)</f>
+        <v>0.82996222222222205</v>
+      </c>
+      <c r="D109">
+        <f t="shared" ref="D109:J109" si="27">AVERAGE(D65:D69)</f>
+        <v>0.83058022222222172</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="27"/>
+        <v>0.83061782222222169</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="27"/>
+        <v>0.83105855555555519</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="27"/>
+        <v>0.91762266666666614</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="27"/>
+        <v>0.2711095999999994</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="27"/>
+        <v>0.40883133333333299</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="27"/>
+        <v>0.67529833333333278</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>133</v>
+      </c>
+      <c r="C110">
+        <f>MEDIAN(C65:C69)</f>
+        <v>0.82996222222222205</v>
+      </c>
+      <c r="D110">
+        <f t="shared" ref="D110:J110" si="28">MEDIAN(D65:D69)</f>
+        <v>0.83043722222222205</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="28"/>
+        <v>0.83076855555555496</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="28"/>
+        <v>0.83102933333333295</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="28"/>
+        <v>0.91762266666666603</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="28"/>
+        <v>0.27216333333333298</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="28"/>
+        <v>0.422279388888888</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="28"/>
+        <v>0.66893855555555504</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>134</v>
+      </c>
+      <c r="C111">
+        <f>_xlfn.STDEV.S(C65:C69)</f>
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <f t="shared" ref="D111:J111" si="29">_xlfn.STDEV.S(D65:D69)</f>
+        <v>8.9008755638123451E-4</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="29"/>
+        <v>5.9254282858195819E-4</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="29"/>
+        <v>4.0575153560011009E-4</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="29"/>
+        <v>5.2073741198789322E-3</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="29"/>
+        <v>3.8185938141910021E-2</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="29"/>
+        <v>3.4462572485627917E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:J69">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>C2=MAX($C2:$J2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4150,10 +5484,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B2940F-B4D6-41E5-A124-BC142EFBCEFB}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="L110" sqref="L110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5801,9 +7135,1165 @@
         <v>0.57926066666666598</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73">
+        <f>AVERAGE(C2:C6)</f>
+        <v>0.40520133333333302</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ref="D73:J73" si="0">AVERAGE(D2:D6)</f>
+        <v>0.40517668888888869</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="0"/>
+        <v>0.40518319999999941</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="0"/>
+        <v>0.4051695999999998</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="0"/>
+        <v>0.43255566666666601</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="0"/>
+        <v>0.41694306666666614</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="0"/>
+        <v>0.43331367777777735</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="0"/>
+        <v>0.5788088666666662</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74">
+        <f>MEDIAN(C2:C6)</f>
+        <v>0.40520133333333302</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ref="D74:J74" si="1">MEDIAN(D2:D6)</f>
+        <v>0.40518111111111099</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>0.40516855555555498</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>0.40516333333333299</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>0.43255566666666601</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>0.428419555555555</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="1"/>
+        <v>0.43893822222222201</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>0.58401377777777697</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>134</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f>_xlfn.STDEV.S(D2:D6)</f>
+        <v>1.2150965007648371E-4</v>
+      </c>
+      <c r="E75">
+        <f t="shared" ref="E75:J75" si="2">_xlfn.STDEV.S(E2:E6)</f>
+        <v>5.8500416796858792E-5</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="2"/>
+        <v>3.173429425870788E-5</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="2"/>
+        <v>2.02069075028645E-2</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="2"/>
+        <v>1.4520801281722685E-2</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="2"/>
+        <v>6.4464419386861552E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77">
+        <f>AVERAGE(C9:C13)</f>
+        <v>0.68518900000000005</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77:J77" si="3">AVERAGE(D9:D13)</f>
+        <v>0.68503904444444397</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>0.68504479999999934</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>0.68502533333333282</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="3"/>
+        <v>0.688974444444444</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="3"/>
+        <v>0.34987742222222196</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="3"/>
+        <v>0.36505895555555518</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="3"/>
+        <v>0.500022844444444</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>133</v>
+      </c>
+      <c r="C78">
+        <f>MEDIAN(C9:C13)</f>
+        <v>0.68518900000000005</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ref="D78:J78" si="4">MEDIAN(D9:D13)</f>
+        <v>0.68511444444444403</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="4"/>
+        <v>0.68503888888888798</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="4"/>
+        <v>0.68502377777777701</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>0.688974444444444</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="4"/>
+        <v>0.35101894444444398</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="4"/>
+        <v>0.36267305555555501</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="4"/>
+        <v>0.492720555555555</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79">
+        <f>_xlfn.STDEV.S(C9:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <f>_xlfn.STDEV.S(D9:D13)</f>
+        <v>1.8374654779661201E-4</v>
+      </c>
+      <c r="E79">
+        <f t="shared" ref="D79:J79" si="5">_xlfn.STDEV.S(E9:E13)</f>
+        <v>1.4691196658528588E-4</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="5"/>
+        <v>3.632432779990085E-5</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="5"/>
+        <v>2.1003889180780701E-2</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="5"/>
+        <v>5.4589786834213947E-3</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="5"/>
+        <v>1.5297455550668835E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81">
+        <f>AVERAGE(C16:C20)</f>
+        <v>0.517665777777777</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ref="D81:J81" si="6">AVERAGE(D16:D20)</f>
+        <v>0.51747737777777714</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>0.51743866666666616</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="6"/>
+        <v>0.51746782222222187</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="6"/>
+        <v>0.50465244444444401</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="6"/>
+        <v>0.47085834444444374</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="6"/>
+        <v>0.49831421111111052</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="6"/>
+        <v>0.53805535555555528</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82">
+        <f>MEDIAN(C16:C20)</f>
+        <v>0.517665777777777</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ref="D82:J82" si="7">MEDIAN(D16:D20)</f>
+        <v>0.51746422222222199</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="7"/>
+        <v>0.51748577777777705</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="7"/>
+        <v>0.51746411111111101</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="7"/>
+        <v>0.50465244444444401</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="7"/>
+        <v>0.47051483333333299</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="7"/>
+        <v>0.50071216666666596</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="7"/>
+        <v>0.53784422222222195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83">
+        <f>_xlfn.STDEV.S(C16:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <f t="shared" ref="D83:J83" si="8">_xlfn.STDEV.S(D16:D20)</f>
+        <v>1.8073050669269522E-4</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="8"/>
+        <v>1.8639437812754882E-4</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="8"/>
+        <v>5.7636933032493099E-5</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="8"/>
+        <v>5.1514355965949273E-3</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="8"/>
+        <v>6.7953513025221903E-3</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="8"/>
+        <v>1.5200166207343407E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85">
+        <f>AVERAGE(C23:C27)</f>
+        <v>0.69185177777777696</v>
+      </c>
+      <c r="D85">
+        <f t="shared" ref="D85:J85" si="9">AVERAGE(D23:D27)</f>
+        <v>0.69254604444444379</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="9"/>
+        <v>0.69251917777777738</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="9"/>
+        <v>0.69261088888888833</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="9"/>
+        <v>0.72191899999999998</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="9"/>
+        <v>0.56223447777777724</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="9"/>
+        <v>0.65191003333333308</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="9"/>
+        <v>0.49859602222222177</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>133</v>
+      </c>
+      <c r="C86">
+        <f>MEDIAN(C23:C27)</f>
+        <v>0.69185177777777696</v>
+      </c>
+      <c r="D86">
+        <f>MEDIAN(D23:D27)</f>
+        <v>0.69251277777777698</v>
+      </c>
+      <c r="E86">
+        <f t="shared" ref="D86:J86" si="10">MEDIAN(E23:E27)</f>
+        <v>0.69252122222222201</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="10"/>
+        <v>0.69258811111111096</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="10"/>
+        <v>0.72191899999999998</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="10"/>
+        <v>0.595766388888888</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="10"/>
+        <v>0.65147911111111101</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="10"/>
+        <v>0.496808444444444</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <f>_xlfn.STDEV.S(D23:D27)</f>
+        <v>1.8214194708758482E-4</v>
+      </c>
+      <c r="E87">
+        <f t="shared" ref="E87:J87" si="11">_xlfn.STDEV.S(E23:E27)</f>
+        <v>8.1677421816433342E-5</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="11"/>
+        <v>1.0303385515766536E-4</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="11"/>
+        <v>6.4705999714515738E-2</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="11"/>
+        <v>4.8498367621759072E-3</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="11"/>
+        <v>6.9373174154150419E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89">
+        <f>AVERAGE(C30:C34)</f>
+        <v>0.51083355555555499</v>
+      </c>
+      <c r="D89">
+        <f t="shared" ref="D89:J89" si="12">AVERAGE(D30:D34)</f>
+        <v>0.51093259999999963</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="12"/>
+        <v>0.5108902222222218</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="12"/>
+        <v>0.5109692444444438</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="12"/>
+        <v>0.49463538888888803</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="12"/>
+        <v>0.48512495555555518</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="12"/>
+        <v>0.509193155555555</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="12"/>
+        <v>0.52083765555555495</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90">
+        <f>MEDIAN(C30:C34)</f>
+        <v>0.51083355555555499</v>
+      </c>
+      <c r="D90">
+        <f t="shared" ref="D90:J90" si="13">MEDIAN(D30:D34)</f>
+        <v>0.51088188888888797</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="13"/>
+        <v>0.51090277777777704</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="13"/>
+        <v>0.510957555555555</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="13"/>
+        <v>0.49463538888888797</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="13"/>
+        <v>0.48215405555555502</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="13"/>
+        <v>0.51078722222222195</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="13"/>
+        <v>0.51445244444444405</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91">
+        <f>_xlfn.STDEV.S(C30:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <f t="shared" ref="D91:J91" si="14">_xlfn.STDEV.S(D30:D34)</f>
+        <v>1.5157587025802212E-4</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="14"/>
+        <v>1.515974404488812E-4</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="14"/>
+        <v>1.1007335937670645E-4</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="14"/>
+        <v>6.2063353831181828E-17</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="14"/>
+        <v>8.6541003738968263E-3</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="14"/>
+        <v>4.2103783995731843E-3</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="14"/>
+        <v>3.3290984460478922E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>132</v>
+      </c>
+      <c r="C93">
+        <f>AVERAGE(C37:C41)</f>
+        <v>0.688305888888888</v>
+      </c>
+      <c r="D93">
+        <f t="shared" ref="D93:J93" si="15">AVERAGE(D37:D41)</f>
+        <v>0.68825106666666613</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="15"/>
+        <v>0.68819115555555521</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="15"/>
+        <v>0.6882223333333326</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="15"/>
+        <v>0.765905888888888</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="15"/>
+        <v>0.56000402222222179</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="15"/>
+        <v>0.63521946666666618</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="15"/>
+        <v>0.50499692222222214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>133</v>
+      </c>
+      <c r="C94">
+        <f>MEDIAN(C37:C41)</f>
+        <v>0.688305888888888</v>
+      </c>
+      <c r="D94">
+        <f t="shared" ref="D94:J94" si="16">MEDIAN(D37:D41)</f>
+        <v>0.68826733333333301</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="16"/>
+        <v>0.68821711111111095</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="16"/>
+        <v>0.68819388888888799</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="16"/>
+        <v>0.765905888888888</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="16"/>
+        <v>0.55607961111111104</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="16"/>
+        <v>0.63399366666666601</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="16"/>
+        <v>0.50550050000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95">
+        <f>_xlfn.STDEV.S(C37:C41)</f>
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <f t="shared" ref="D95:J95" si="17">_xlfn.STDEV.S(D37:D41)</f>
+        <v>1.3026811383236349E-4</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="17"/>
+        <v>7.266499318492751E-5</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="17"/>
+        <v>7.2284801947556811E-5</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="17"/>
+        <v>1.1286588249998368E-2</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="17"/>
+        <v>1.0424579641923514E-2</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="17"/>
+        <v>7.3784041063627657E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97">
+        <f>AVERAGE(C44:C48)</f>
+        <v>0.50621899999999997</v>
+      </c>
+      <c r="D97">
+        <f t="shared" ref="D97:J97" si="18">AVERAGE(D44:D48)</f>
+        <v>0.50721466666666615</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="18"/>
+        <v>0.50715599999999961</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="18"/>
+        <v>0.50723426666666627</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="18"/>
+        <v>0.50651500000000005</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="18"/>
+        <v>0.54185781111111075</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="18"/>
+        <v>0.55215812222222205</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="18"/>
+        <v>0.51798704444444377</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>133</v>
+      </c>
+      <c r="C98">
+        <f>MEDIAN(C44:C48)</f>
+        <v>0.50621899999999997</v>
+      </c>
+      <c r="D98">
+        <f t="shared" ref="D98:J98" si="19">MEDIAN(D44:D48)</f>
+        <v>0.50719433333333297</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="19"/>
+        <v>0.50711300000000004</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="19"/>
+        <v>0.50724599999999997</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="19"/>
+        <v>0.50651500000000005</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="19"/>
+        <v>0.54363344444444395</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="19"/>
+        <v>0.55384955555555504</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="19"/>
+        <v>0.52042277777777701</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99">
+        <f>_xlfn.STDEV.S(C44:C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <f t="shared" ref="D99:J99" si="20">_xlfn.STDEV.S(D44:D48)</f>
+        <v>1.0132379950286831E-4</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="20"/>
+        <v>1.3234543745348576E-4</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="20"/>
+        <v>8.0805688285521605E-5</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="20"/>
+        <v>5.5771241106024275E-3</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="20"/>
+        <v>4.8883716685683073E-3</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="20"/>
+        <v>6.9829131836175009E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>132</v>
+      </c>
+      <c r="C101">
+        <f>AVERAGE(C51:C55)</f>
+        <v>0.64907433333333298</v>
+      </c>
+      <c r="D101">
+        <f>AVERAGE(D51:D55)</f>
+        <v>0.64875213333333304</v>
+      </c>
+      <c r="E101">
+        <f t="shared" ref="D101:J101" si="21">AVERAGE(E51:E55)</f>
+        <v>0.64877231111111078</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="21"/>
+        <v>0.64886102222222186</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="21"/>
+        <v>0.67549611111111096</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="21"/>
+        <v>0.51910996666666631</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="21"/>
+        <v>0.52719151111111073</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="21"/>
+        <v>0.49046458888888855</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>133</v>
+      </c>
+      <c r="C102">
+        <f>MEDIAN(C51:C55)</f>
+        <v>0.64907433333333298</v>
+      </c>
+      <c r="D102">
+        <f t="shared" ref="D102:J102" si="22">MEDIAN(D51:D55)</f>
+        <v>0.64877688888888896</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="22"/>
+        <v>0.64878022222222198</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="22"/>
+        <v>0.64886888888888805</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="22"/>
+        <v>0.67549611111111096</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="22"/>
+        <v>0.52163649999999995</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="22"/>
+        <v>0.52804477777777703</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="22"/>
+        <v>0.48700399999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>134</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <f>_xlfn.STDEV.S(D51:D55)</f>
+        <v>7.4229681926921815E-5</v>
+      </c>
+      <c r="E103">
+        <f t="shared" ref="E103:J103" si="23">_xlfn.STDEV.S(E51:E55)</f>
+        <v>6.3428213530089433E-5</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="23"/>
+        <v>7.4038753615930915E-5</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="23"/>
+        <v>6.2588739685601339E-3</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="23"/>
+        <v>7.7840225751017655E-3</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="23"/>
+        <v>1.6656722786151316E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>132</v>
+      </c>
+      <c r="C105">
+        <f>AVERAGE(C58:C62)</f>
+        <v>0.43983988888888803</v>
+      </c>
+      <c r="D105">
+        <f t="shared" ref="D105:J105" si="24">AVERAGE(D58:D62)</f>
+        <v>0.43965284444444375</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="24"/>
+        <v>0.43963588888888838</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="24"/>
+        <v>0.43959455555555521</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="24"/>
+        <v>0.43535877777777704</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="24"/>
+        <v>0.53675424444444397</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="24"/>
+        <v>0.54374944444444395</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="24"/>
+        <v>0.55618364444444379</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>133</v>
+      </c>
+      <c r="C106">
+        <f>MEDIAN(C58:C62)</f>
+        <v>0.43983988888888798</v>
+      </c>
+      <c r="D106">
+        <f>MEDIAN(D58:D62)</f>
+        <v>0.43975488888888797</v>
+      </c>
+      <c r="E106">
+        <f t="shared" ref="D106:J106" si="25">MEDIAN(E58:E62)</f>
+        <v>0.43960966666666601</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="25"/>
+        <v>0.43957444444444399</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="25"/>
+        <v>0.43535877777777698</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="25"/>
+        <v>0.53904716666666597</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="25"/>
+        <v>0.54597027777777696</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="25"/>
+        <v>0.56947594444444405</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>134</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <f>_xlfn.STDEV.S(D58:D62)</f>
+        <v>1.8776108735796656E-4</v>
+      </c>
+      <c r="E107">
+        <f t="shared" ref="E107:J107" si="26">_xlfn.STDEV.S(E58:E62)</f>
+        <v>1.3036655350060131E-4</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="26"/>
+        <v>5.0404536342911856E-5</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="26"/>
+        <v>6.2063353831181828E-17</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="26"/>
+        <v>1.3379833021665895E-2</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="26"/>
+        <v>4.6593657219148998E-3</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="26"/>
+        <v>3.9636506394930542E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>132</v>
+      </c>
+      <c r="C109">
+        <f>AVERAGE(C65:C69)</f>
+        <v>0.66053311111111102</v>
+      </c>
+      <c r="D109">
+        <f t="shared" ref="D109:J109" si="27">AVERAGE(D65:D69)</f>
+        <v>0.66107822222222157</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="27"/>
+        <v>0.66106597777777765</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="27"/>
+        <v>0.66107715555555502</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="27"/>
+        <v>0.67925322222222195</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="27"/>
+        <v>0.39422634444444399</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="27"/>
+        <v>0.28498229999999963</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="27"/>
+        <v>0.51012408888888838</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>133</v>
+      </c>
+      <c r="C110">
+        <f>MEDIAN(C65:C69)</f>
+        <v>0.66053311111111102</v>
+      </c>
+      <c r="D110">
+        <f t="shared" ref="D110:J110" si="28">MEDIAN(D65:D69)</f>
+        <v>0.66115877777777698</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="28"/>
+        <v>0.66103033333333305</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="28"/>
+        <v>0.661092666666666</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="28"/>
+        <v>0.67925322222222195</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="28"/>
+        <v>0.39754027777777701</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="28"/>
+        <v>0.28691361111111102</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="28"/>
+        <v>0.51372477777777703</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>134</v>
+      </c>
+      <c r="C111">
+        <f>_xlfn.STDEV.S(C65:C69)</f>
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <f t="shared" ref="D111:J111" si="29">_xlfn.STDEV.S(D65:D69)</f>
+        <v>2.0964923674830879E-4</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="29"/>
+        <v>1.256821240123666E-4</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="29"/>
+        <v>7.8351873298307593E-5</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="29"/>
+        <v>1.9793819685559443E-2</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="29"/>
+        <v>8.2457017245313232E-3</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="29"/>
+        <v>7.4843044290042557E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:J69">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>C2=MAX($C2:$J2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6481,10 +8971,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B22AB39-7364-4596-83A8-2C3979A060DF}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6580,9 +9070,36 @@
         <v>0.68878561111111103</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(Tabelle11[Test AUC])</f>
+        <v>0.61374167777777733</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14">
+        <f>MEDIAN(Tabelle11[Test AUC])</f>
+        <v>0.60359522222222151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15">
+        <f>_xlfn.STDEV.S(Tabelle11[Test AUC])</f>
+        <v>7.7554432319688088E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>B2=MAX(B$2:B$11)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6896,10 +9413,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66800C28-627D-4DD7-A496-EC282D19DD96}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6995,9 +9512,36 @@
         <v>0.96254441866158602</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(Tabelle13[Test AUC])</f>
+        <v>0.93057611521195371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14">
+        <f>MEDIAN(Tabelle13[Test AUC])</f>
+        <v>0.93870175532329547</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15">
+        <f>_xlfn.STDEV.S(Tabelle13[Test AUC])</f>
+        <v>4.7098392080479258E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>B2=MAX(B$2:B$11)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7010,10 +9554,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475F6751-152A-4EE3-A1A4-9980A8DC1197}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C16"/>
+      <selection activeCell="B22" sqref="A20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7199,14 +9743,41 @@
         <v>0.414871122222222</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(Tabelle_Params_8_C__2[[ Average AUC]])</f>
+        <v>0.3306368118518514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21">
+        <f>MEDIAN(Tabelle_Params_8_C__2[[ Average AUC]])</f>
+        <v>0.33435933333333301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22">
+        <f>_xlfn.STDEV.S(Tabelle_Params_8_C__2[[ Average AUC]])</f>
+        <v>6.7474406074188142E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>C2=MAX(C$2:C$16)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7219,10 +9790,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1713303F-87FE-4205-B3EA-701B76971E5A}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C16"/>
+      <selection activeCell="B22" sqref="A20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7408,14 +9979,41 @@
         <v>0.55700373333333297</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>92</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(Tabelle_Params_6_C[[ Average AUC]])</f>
+        <v>0.5573014392592589</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21">
+        <f>MEDIAN(Tabelle_Params_6_C[[ Average AUC]])</f>
+        <v>0.57118539999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22">
+        <f>_xlfn.STDEV.S(Tabelle_Params_6_C[[ Average AUC]])</f>
+        <v>5.8672201864228772E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>C2=MAX(C$2:C$16)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7428,10 +10026,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77925A-1F00-4EC3-943E-6E01C2893086}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="B16" sqref="A14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7554,6 +10152,33 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(Tabelle_Params_8_F[[ AUC]])</f>
+        <v>0.58872510493827124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15">
+        <f>MEDIAN(Tabelle_Params_8_F[[ AUC]])</f>
+        <v>0.68701322222222205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16">
+        <f>_xlfn.STDEV.S(Tabelle_Params_8_F[[ AUC]])</f>
+        <v>0.16892334526131716</v>
       </c>
     </row>
   </sheetData>
@@ -7571,10 +10196,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C94A5B2-E82A-495F-9CAA-DD30ADD2B5A6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7699,9 +10324,36 @@
         <v>77</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(Tabelle_Params_8_C[AUC])</f>
+        <v>0.55133427777777722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15">
+        <f>MEDIAN(Tabelle_Params_8_C[AUC])</f>
+        <v>0.645905888888888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16">
+        <f>_xlfn.STDEV.S(Tabelle_Params_8_C[AUC])</f>
+        <v>0.1421713314917048</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>C2=MAX(C$2:C$10)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7714,10 +10366,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A602A0DE-CDA1-4987-A592-0C47634656C6}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="B2:I6"/>
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7904,9 +10556,120 @@
         <v>0.609111576428357</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(Tabelle_Waveform[LOF_AUC])</f>
+        <v>0.73067603948549198</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(Tabelle_Waveform[LOF_50])</f>
+        <v>0.73492850732874637</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(Tabelle_Waveform[LOF_100])</f>
+        <v>0.73646126233921583</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(Tabelle_Waveform[LOF_500])</f>
+        <v>0.7355088244092125</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(Tabelle_Waveform[KNN_AUC])</f>
+        <v>0.73459018845348401</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(Tabelle_Waveform[MO_GAAL_AUC])</f>
+        <v>0.40652378103499798</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(Tabelle_Waveform[AnoGAN_AUC])</f>
+        <v>0.56582261441818704</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(Tabelle_Waveform[Deep_SVDD_AUC])</f>
+        <v>0.59068022734071168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <f>MEDIAN(Tabelle_Waveform[LOF_AUC])</f>
+        <v>0.73067603948549198</v>
+      </c>
+      <c r="C9">
+        <f>MEDIAN(Tabelle_Waveform[LOF_50])</f>
+        <v>0.735183966497158</v>
+      </c>
+      <c r="D9">
+        <f>MEDIAN(Tabelle_Waveform[LOF_100])</f>
+        <v>0.73625486090337999</v>
+      </c>
+      <c r="E9">
+        <f>MEDIAN(Tabelle_Waveform[LOF_500])</f>
+        <v>0.73583308405623604</v>
+      </c>
+      <c r="F9">
+        <f>MEDIAN(Tabelle_Waveform[KNN_AUC])</f>
+        <v>0.73459018845348401</v>
+      </c>
+      <c r="G9">
+        <f>MEDIAN(Tabelle_Waveform[MO_GAAL_AUC])</f>
+        <v>0.42171402931498603</v>
+      </c>
+      <c r="H9">
+        <f>MEDIAN(Tabelle_Waveform[AnoGAN_AUC])</f>
+        <v>0.54650912354172898</v>
+      </c>
+      <c r="I9">
+        <f>MEDIAN(Tabelle_Waveform[Deep_SVDD_AUC])</f>
+        <v>0.60106790308106495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[LOF_AUC])</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[LOF_50])</f>
+        <v>1.9733754150247718E-3</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[LOF_100])</f>
+        <v>8.7015175721404624E-4</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[LOF_500])</f>
+        <v>1.2011159501961086E-3</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[KNN_AUC])</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[MO_GAAL_AUC])</f>
+        <v>0.11560382621808973</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[AnoGAN_AUC])</f>
+        <v>0.10097690169516349</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.STDEV.S(Tabelle_Waveform[Deep_SVDD_AUC])</f>
+        <v>4.2062439671242971E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:I6">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>B2=MAX($B2:$I2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7919,10 +10682,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA25CDC-A440-49FC-875A-810888E3A18E}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C8" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8108,9 +10871,118 @@
         <v>0.72109239265326397</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(Tabelle_Spambase[LOF_AUC])</f>
+        <v>0.82935436832961007</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(Tabelle_Spambase[LOF_50])</f>
+        <v>0.76659530900967932</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(Tabelle_Spambase[LOF_100])</f>
+        <v>0.74113303549267762</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(Tabelle_Spambase[LOF_500])</f>
+        <v>0.67732843137254828</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(Tabelle_Spambase[KNN_AUC])</f>
+        <v>0.80558528791263284</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(Tabelle_Spambase[MO_GAAL_AUC])</f>
+        <v>0.383814221891288</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(Tabelle_Spambase[AnoGAN_AUC])</f>
+        <v>0.60665642839414224</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(Tabelle_Spambase[Deep_SVDD_AUC])</f>
+        <v>0.68467982129560634</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <f>MEDIAN(Tabelle_Spambase[LOF_AUC])</f>
+        <v>0.82935436832960996</v>
+      </c>
+      <c r="C9">
+        <f>MEDIAN(Tabelle_Spambase[LOF_50])</f>
+        <v>0.76330199801439502</v>
+      </c>
+      <c r="D9">
+        <f>MEDIAN(Tabelle_Spambase[LOF_100])</f>
+        <v>0.74498945147679296</v>
+      </c>
+      <c r="E9">
+        <f>MEDIAN(Tabelle_Spambase[LOF_500])</f>
+        <v>0.67429107719036896</v>
+      </c>
+      <c r="F9">
+        <f>MEDIAN(Tabelle_Spambase[KNN_AUC])</f>
+        <v>0.80558528791263295</v>
+      </c>
+      <c r="G9">
+        <f>MEDIAN(Tabelle_Spambase[MO_GAAL_AUC])</f>
+        <v>0.38462552742616002</v>
+      </c>
+      <c r="H9">
+        <f>MEDIAN(Tabelle_Spambase[AnoGAN_AUC])</f>
+        <v>0.66389767932489396</v>
+      </c>
+      <c r="I9">
+        <f>MEDIAN(Tabelle_Spambase[Deep_SVDD_AUC])</f>
+        <v>0.68003071481757205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.STDEV.S(Tabelle_Spambase[LOF_50])</f>
+        <v>1.5733044867305871E-2</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.STDEV.S(Tabelle_Spambase[LOF_100])</f>
+        <v>1.4848771557968488E-2</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.STDEV.S(Tabelle_Spambase[LOF_500])</f>
+        <v>1.5596480519738814E-2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.STDEV.S(Tabelle_Spambase[MO_GAAL_AUC])</f>
+        <v>3.6348999212609298E-2</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.STDEV.S(Tabelle_Spambase[AnoGAN_AUC])</f>
+        <v>0.16199930611884092</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.STDEV.S(Tabelle_Spambase[Deep_SVDD_AUC])</f>
+        <v>3.198948190420435E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:I6">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>B2=MAX($B2:$I2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>